<commit_message>
Fix Railway build: remove nixpacks phases, lock Node 20
</commit_message>
<xml_diff>
--- a/SurgePure NPI New Products Template 2026-01-19 (1).xlsx
+++ b/SurgePure NPI New Products Template 2026-01-19 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Product Marketing\Ryan\NPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anisurrahman/Projects/partly_v11_vsurgepure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E3ED958-3B10-4A0C-ADC2-06B6FEE33408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E397DE0-3D68-FC4B-BF39-7928B5E232AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{161EE9C0-EF70-4478-9753-E14F0ED3EF20}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29040" windowHeight="15840" xr2:uid="{161EE9C0-EF70-4478-9753-E14F0ED3EF20}"/>
   </bookViews>
   <sheets>
     <sheet name="NPI LOAD TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -1788,55 +1788,55 @@
   <dimension ref="A1:CC440"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="177.42578125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="2"/>
-    <col min="13" max="13" width="10.85546875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="78.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="177.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="2"/>
+    <col min="13" max="13" width="10.83203125" style="9" customWidth="1"/>
     <col min="14" max="14" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="2"/>
-    <col min="17" max="17" width="7.85546875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="2"/>
+    <col min="17" max="17" width="7.83203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.83203125" style="2" customWidth="1"/>
     <col min="19" max="19" width="8" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" style="2" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="9" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" style="9" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" style="9" customWidth="1"/>
-    <col min="27" max="27" width="9.42578125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="11.140625" style="9" customWidth="1"/>
+    <col min="20" max="20" width="10.5" style="2" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="9.5" style="9" customWidth="1"/>
+    <col min="23" max="23" width="9.5" style="2" customWidth="1"/>
+    <col min="24" max="24" width="10.5" style="9" customWidth="1"/>
+    <col min="25" max="25" width="10.1640625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" style="9" customWidth="1"/>
+    <col min="27" max="27" width="9.5" style="2" customWidth="1"/>
+    <col min="28" max="28" width="11.1640625" style="9" customWidth="1"/>
     <col min="29" max="29" width="9" style="2" customWidth="1"/>
-    <col min="30" max="30" width="10.5703125" style="9" customWidth="1"/>
-    <col min="31" max="31" width="176.42578125" style="8" customWidth="1"/>
-    <col min="32" max="32" width="252.85546875" style="8" customWidth="1"/>
+    <col min="30" max="30" width="10.5" style="9" customWidth="1"/>
+    <col min="31" max="31" width="176.5" style="8" customWidth="1"/>
+    <col min="32" max="32" width="252.83203125" style="8" customWidth="1"/>
     <col min="33" max="33" width="205" style="8" customWidth="1"/>
-    <col min="34" max="34" width="92.140625" style="8" customWidth="1"/>
-    <col min="35" max="35" width="25.5703125" style="2" customWidth="1"/>
-    <col min="36" max="36" width="24.7109375" style="2" customWidth="1"/>
-    <col min="37" max="37" width="16.7109375" style="2" customWidth="1"/>
-    <col min="38" max="38" width="9.42578125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="92.1640625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="25.5" style="2" customWidth="1"/>
+    <col min="36" max="36" width="24.6640625" style="2" customWidth="1"/>
+    <col min="37" max="37" width="16.6640625" style="2" customWidth="1"/>
+    <col min="38" max="38" width="9.5" style="2" customWidth="1"/>
     <col min="39" max="39" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="9.140625" style="1"/>
+    <col min="40" max="40" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>27</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="CB1" s="7"/>
       <c r="CC1" s="7"/>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="2">
         <v>8865</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>8865</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>8865</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>8865</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>8865</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>8865</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>8865</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>8865</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>8865</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>8865</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>8865</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>8865</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>8865</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>8865</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:81" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>8865</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>8865</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>8865</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>8865</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>8865</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>8865</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>8865</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>8865</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>8865</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>8865</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <v>8865</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
         <v>8865</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>8865</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
         <v>8865</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
         <v>8865</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
         <v>8865</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>8865</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
         <v>8865</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="2">
         <v>8865</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="2">
         <v>8865</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="2">
         <v>8865</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="2">
         <v>8865</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
         <v>8865</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
         <v>8865</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
         <v>8865</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
         <v>8865</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="2">
         <v>8865</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="2">
         <v>8865</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="2">
         <v>8865</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="2">
         <v>8865</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="2">
         <v>8865</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="2">
         <v>8865</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="2">
         <v>8865</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="2">
         <v>8865</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
         <v>8865</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
         <v>8865</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="2">
         <v>8865</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="2">
         <v>8865</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="2">
         <v>8865</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" s="2">
         <v>8865</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" s="2">
         <v>8865</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B57" s="2">
         <v>8865</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="2">
         <v>8865</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="2">
         <v>8865</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B60" s="2">
         <v>8865</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B61" s="2">
         <v>8865</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="2">
         <v>8865</v>
       </c>
@@ -7550,7 +7550,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="2">
         <v>8865</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B64" s="2">
         <v>8865</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B65" s="2">
         <v>8865</v>
       </c>
@@ -7823,7 +7823,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B66" s="2">
         <v>8865</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="2">
         <v>8865</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="2">
         <v>8865</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="2">
         <v>8865</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="2">
         <v>8865</v>
       </c>
@@ -8278,7 +8278,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" s="2">
         <v>8865</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="2">
         <v>8865</v>
       </c>
@@ -8460,7 +8460,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B73" s="2">
         <v>8865</v>
       </c>
@@ -8551,7 +8551,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B74" s="2">
         <v>8865</v>
       </c>
@@ -8642,7 +8642,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="2">
         <v>8865</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B76" s="2">
         <v>8865</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B77" s="2">
         <v>8865</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="2">
         <v>8865</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B79" s="2">
         <v>8865</v>
       </c>
@@ -9097,7 +9097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:40" ht="16" x14ac:dyDescent="0.2">
       <c r="B80" s="2">
         <v>8865</v>
       </c>
@@ -9188,7 +9188,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C81" s="11"/>
       <c r="D81"/>
       <c r="E81"/>
@@ -9199,7 +9199,7 @@
       <c r="U81" s="23"/>
       <c r="V81" s="10"/>
     </row>
-    <row r="82" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C82" s="11"/>
       <c r="D82"/>
       <c r="E82"/>
@@ -9210,7 +9210,7 @@
       <c r="U82" s="23"/>
       <c r="V82" s="10"/>
     </row>
-    <row r="83" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C83" s="11"/>
       <c r="D83"/>
       <c r="E83"/>
@@ -9221,7 +9221,7 @@
       <c r="U83" s="23"/>
       <c r="V83" s="10"/>
     </row>
-    <row r="84" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C84" s="11"/>
       <c r="D84"/>
       <c r="E84"/>
@@ -9232,7 +9232,7 @@
       <c r="U84" s="23"/>
       <c r="V84" s="10"/>
     </row>
-    <row r="85" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C85" s="11"/>
       <c r="D85"/>
       <c r="E85"/>
@@ -9243,7 +9243,7 @@
       <c r="U85" s="23"/>
       <c r="V85" s="10"/>
     </row>
-    <row r="86" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C86" s="11"/>
       <c r="D86"/>
       <c r="E86"/>
@@ -9254,7 +9254,7 @@
       <c r="U86" s="23"/>
       <c r="V86" s="10"/>
     </row>
-    <row r="87" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C87" s="11"/>
       <c r="D87"/>
       <c r="E87"/>
@@ -9265,7 +9265,7 @@
       <c r="U87" s="23"/>
       <c r="V87" s="10"/>
     </row>
-    <row r="88" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C88" s="11"/>
       <c r="D88"/>
       <c r="E88"/>
@@ -9276,7 +9276,7 @@
       <c r="U88" s="23"/>
       <c r="V88" s="10"/>
     </row>
-    <row r="89" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C89" s="11"/>
       <c r="D89"/>
       <c r="E89"/>
@@ -9287,7 +9287,7 @@
       <c r="U89" s="23"/>
       <c r="V89" s="10"/>
     </row>
-    <row r="90" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C90" s="11"/>
       <c r="D90"/>
       <c r="E90"/>
@@ -9298,7 +9298,7 @@
       <c r="U90" s="23"/>
       <c r="V90" s="10"/>
     </row>
-    <row r="91" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C91" s="11"/>
       <c r="D91"/>
       <c r="E91"/>
@@ -9309,7 +9309,7 @@
       <c r="U91" s="23"/>
       <c r="V91" s="10"/>
     </row>
-    <row r="92" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C92" s="11"/>
       <c r="D92"/>
       <c r="E92"/>
@@ -9320,7 +9320,7 @@
       <c r="U92" s="23"/>
       <c r="V92" s="10"/>
     </row>
-    <row r="93" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C93" s="11"/>
       <c r="D93"/>
       <c r="E93"/>
@@ -9331,7 +9331,7 @@
       <c r="U93" s="23"/>
       <c r="V93" s="10"/>
     </row>
-    <row r="94" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C94" s="11"/>
       <c r="D94"/>
       <c r="E94"/>
@@ -9342,7 +9342,7 @@
       <c r="U94" s="23"/>
       <c r="V94" s="10"/>
     </row>
-    <row r="95" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C95" s="11"/>
       <c r="D95"/>
       <c r="E95"/>
@@ -9353,7 +9353,7 @@
       <c r="U95" s="23"/>
       <c r="V95" s="10"/>
     </row>
-    <row r="96" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C96" s="11"/>
       <c r="D96"/>
       <c r="E96"/>
@@ -9364,7 +9364,7 @@
       <c r="U96" s="23"/>
       <c r="V96" s="10"/>
     </row>
-    <row r="97" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C97" s="11"/>
       <c r="D97"/>
       <c r="E97"/>
@@ -9375,7 +9375,7 @@
       <c r="U97" s="23"/>
       <c r="V97" s="10"/>
     </row>
-    <row r="98" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C98" s="11"/>
       <c r="D98"/>
       <c r="E98"/>
@@ -9386,7 +9386,7 @@
       <c r="U98" s="23"/>
       <c r="V98" s="10"/>
     </row>
-    <row r="99" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C99" s="11"/>
       <c r="D99"/>
       <c r="E99"/>
@@ -9397,7 +9397,7 @@
       <c r="U99" s="23"/>
       <c r="V99" s="10"/>
     </row>
-    <row r="100" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C100" s="11"/>
       <c r="D100"/>
       <c r="E100"/>
@@ -9408,7 +9408,7 @@
       <c r="U100" s="23"/>
       <c r="V100" s="10"/>
     </row>
-    <row r="101" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C101" s="11"/>
       <c r="D101"/>
       <c r="E101"/>
@@ -9419,7 +9419,7 @@
       <c r="U101" s="23"/>
       <c r="V101" s="10"/>
     </row>
-    <row r="102" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C102" s="11"/>
       <c r="D102"/>
       <c r="E102"/>
@@ -9430,7 +9430,7 @@
       <c r="U102" s="23"/>
       <c r="V102" s="10"/>
     </row>
-    <row r="103" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C103" s="11"/>
       <c r="D103"/>
       <c r="E103"/>
@@ -9441,7 +9441,7 @@
       <c r="U103" s="23"/>
       <c r="V103" s="10"/>
     </row>
-    <row r="104" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C104" s="11"/>
       <c r="D104"/>
       <c r="E104"/>
@@ -9452,7 +9452,7 @@
       <c r="U104" s="23"/>
       <c r="V104" s="10"/>
     </row>
-    <row r="105" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C105" s="11"/>
       <c r="D105"/>
       <c r="E105"/>
@@ -9463,7 +9463,7 @@
       <c r="U105" s="23"/>
       <c r="V105" s="10"/>
     </row>
-    <row r="106" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C106" s="11"/>
       <c r="D106"/>
       <c r="E106"/>
@@ -9474,7 +9474,7 @@
       <c r="U106" s="23"/>
       <c r="V106" s="10"/>
     </row>
-    <row r="107" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C107" s="11"/>
       <c r="D107"/>
       <c r="E107"/>
@@ -9485,7 +9485,7 @@
       <c r="U107" s="23"/>
       <c r="V107" s="10"/>
     </row>
-    <row r="108" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C108" s="11"/>
       <c r="D108"/>
       <c r="E108"/>
@@ -9496,7 +9496,7 @@
       <c r="U108" s="23"/>
       <c r="V108" s="10"/>
     </row>
-    <row r="109" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C109" s="11"/>
       <c r="D109"/>
       <c r="E109"/>
@@ -9507,7 +9507,7 @@
       <c r="U109" s="23"/>
       <c r="V109" s="10"/>
     </row>
-    <row r="110" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C110" s="11"/>
       <c r="D110"/>
       <c r="E110"/>
@@ -9518,7 +9518,7 @@
       <c r="U110" s="23"/>
       <c r="V110" s="10"/>
     </row>
-    <row r="111" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C111" s="11"/>
       <c r="D111"/>
       <c r="E111"/>
@@ -9529,7 +9529,7 @@
       <c r="U111" s="23"/>
       <c r="V111" s="10"/>
     </row>
-    <row r="112" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C112" s="11"/>
       <c r="D112"/>
       <c r="E112"/>
@@ -9540,7 +9540,7 @@
       <c r="U112" s="23"/>
       <c r="V112" s="10"/>
     </row>
-    <row r="113" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C113" s="11"/>
       <c r="D113"/>
       <c r="E113"/>
@@ -9551,7 +9551,7 @@
       <c r="U113" s="23"/>
       <c r="V113" s="10"/>
     </row>
-    <row r="114" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C114" s="11"/>
       <c r="D114"/>
       <c r="E114"/>
@@ -9562,7 +9562,7 @@
       <c r="U114" s="23"/>
       <c r="V114" s="10"/>
     </row>
-    <row r="115" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C115" s="11"/>
       <c r="D115"/>
       <c r="E115"/>
@@ -9573,7 +9573,7 @@
       <c r="U115" s="23"/>
       <c r="V115" s="10"/>
     </row>
-    <row r="116" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C116" s="11"/>
       <c r="D116"/>
       <c r="E116"/>
@@ -9584,7 +9584,7 @@
       <c r="U116" s="23"/>
       <c r="V116" s="10"/>
     </row>
-    <row r="117" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C117" s="11"/>
       <c r="D117"/>
       <c r="E117"/>
@@ -9595,7 +9595,7 @@
       <c r="U117" s="23"/>
       <c r="V117" s="10"/>
     </row>
-    <row r="118" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C118" s="11"/>
       <c r="D118"/>
       <c r="E118"/>
@@ -9606,7 +9606,7 @@
       <c r="U118" s="23"/>
       <c r="V118" s="10"/>
     </row>
-    <row r="119" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C119" s="11"/>
       <c r="D119"/>
       <c r="E119"/>
@@ -9617,7 +9617,7 @@
       <c r="U119" s="23"/>
       <c r="V119" s="10"/>
     </row>
-    <row r="120" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C120" s="11"/>
       <c r="D120"/>
       <c r="E120"/>
@@ -9628,7 +9628,7 @@
       <c r="U120" s="23"/>
       <c r="V120" s="10"/>
     </row>
-    <row r="121" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C121" s="11"/>
       <c r="D121"/>
       <c r="E121"/>
@@ -9639,7 +9639,7 @@
       <c r="U121" s="23"/>
       <c r="V121" s="10"/>
     </row>
-    <row r="122" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C122" s="11"/>
       <c r="D122"/>
       <c r="E122"/>
@@ -9650,7 +9650,7 @@
       <c r="U122" s="23"/>
       <c r="V122" s="10"/>
     </row>
-    <row r="123" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C123" s="11"/>
       <c r="D123"/>
       <c r="E123"/>
@@ -9661,7 +9661,7 @@
       <c r="U123" s="23"/>
       <c r="V123" s="10"/>
     </row>
-    <row r="124" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C124" s="11"/>
       <c r="D124"/>
       <c r="E124"/>
@@ -9672,7 +9672,7 @@
       <c r="U124" s="23"/>
       <c r="V124" s="10"/>
     </row>
-    <row r="125" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C125" s="11"/>
       <c r="D125"/>
       <c r="E125"/>
@@ -9683,7 +9683,7 @@
       <c r="U125" s="23"/>
       <c r="V125" s="10"/>
     </row>
-    <row r="126" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C126" s="11"/>
       <c r="D126"/>
       <c r="E126"/>
@@ -9694,7 +9694,7 @@
       <c r="U126" s="23"/>
       <c r="V126" s="10"/>
     </row>
-    <row r="127" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C127" s="11"/>
       <c r="D127"/>
       <c r="E127"/>
@@ -9705,7 +9705,7 @@
       <c r="U127" s="23"/>
       <c r="V127" s="10"/>
     </row>
-    <row r="128" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C128" s="11"/>
       <c r="D128"/>
       <c r="E128"/>
@@ -9716,7 +9716,7 @@
       <c r="U128" s="23"/>
       <c r="V128" s="10"/>
     </row>
-    <row r="129" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C129" s="11"/>
       <c r="D129"/>
       <c r="E129"/>
@@ -9727,7 +9727,7 @@
       <c r="U129" s="23"/>
       <c r="V129" s="10"/>
     </row>
-    <row r="130" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C130" s="11"/>
       <c r="D130"/>
       <c r="E130"/>
@@ -9738,7 +9738,7 @@
       <c r="U130" s="23"/>
       <c r="V130" s="10"/>
     </row>
-    <row r="131" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C131" s="11"/>
       <c r="D131"/>
       <c r="E131"/>
@@ -9749,7 +9749,7 @@
       <c r="U131" s="23"/>
       <c r="V131" s="10"/>
     </row>
-    <row r="132" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C132" s="11"/>
       <c r="D132"/>
       <c r="E132"/>
@@ -9760,7 +9760,7 @@
       <c r="U132" s="23"/>
       <c r="V132" s="10"/>
     </row>
-    <row r="133" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C133" s="11"/>
       <c r="D133"/>
       <c r="E133"/>
@@ -9771,7 +9771,7 @@
       <c r="U133" s="23"/>
       <c r="V133" s="10"/>
     </row>
-    <row r="134" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C134" s="11"/>
       <c r="D134"/>
       <c r="E134"/>
@@ -9782,7 +9782,7 @@
       <c r="U134" s="23"/>
       <c r="V134" s="10"/>
     </row>
-    <row r="135" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C135" s="11"/>
       <c r="D135"/>
       <c r="E135"/>
@@ -9793,7 +9793,7 @@
       <c r="U135" s="23"/>
       <c r="V135" s="10"/>
     </row>
-    <row r="136" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C136" s="11"/>
       <c r="D136"/>
       <c r="E136"/>
@@ -9804,7 +9804,7 @@
       <c r="U136" s="23"/>
       <c r="V136" s="10"/>
     </row>
-    <row r="137" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C137" s="11"/>
       <c r="D137"/>
       <c r="E137"/>
@@ -9815,7 +9815,7 @@
       <c r="U137" s="23"/>
       <c r="V137" s="10"/>
     </row>
-    <row r="138" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C138" s="11"/>
       <c r="D138"/>
       <c r="E138"/>
@@ -9826,7 +9826,7 @@
       <c r="U138" s="23"/>
       <c r="V138" s="10"/>
     </row>
-    <row r="139" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C139" s="11"/>
       <c r="D139"/>
       <c r="E139"/>
@@ -9837,7 +9837,7 @@
       <c r="U139" s="23"/>
       <c r="V139" s="10"/>
     </row>
-    <row r="140" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C140" s="11"/>
       <c r="D140"/>
       <c r="E140"/>
@@ -9848,7 +9848,7 @@
       <c r="U140" s="23"/>
       <c r="V140" s="10"/>
     </row>
-    <row r="141" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C141" s="11"/>
       <c r="D141"/>
       <c r="E141"/>
@@ -9859,7 +9859,7 @@
       <c r="U141" s="23"/>
       <c r="V141" s="10"/>
     </row>
-    <row r="142" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C142" s="11"/>
       <c r="D142"/>
       <c r="E142"/>
@@ -9870,7 +9870,7 @@
       <c r="U142" s="23"/>
       <c r="V142" s="10"/>
     </row>
-    <row r="143" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C143" s="11"/>
       <c r="D143"/>
       <c r="E143"/>
@@ -9881,7 +9881,7 @@
       <c r="U143" s="23"/>
       <c r="V143" s="10"/>
     </row>
-    <row r="144" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C144" s="11"/>
       <c r="D144"/>
       <c r="E144"/>
@@ -9892,7 +9892,7 @@
       <c r="U144" s="23"/>
       <c r="V144" s="10"/>
     </row>
-    <row r="145" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C145" s="11"/>
       <c r="D145"/>
       <c r="E145"/>
@@ -9903,7 +9903,7 @@
       <c r="U145" s="23"/>
       <c r="V145" s="10"/>
     </row>
-    <row r="146" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C146" s="11"/>
       <c r="D146"/>
       <c r="E146"/>
@@ -9914,7 +9914,7 @@
       <c r="U146" s="23"/>
       <c r="V146" s="10"/>
     </row>
-    <row r="147" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C147" s="11"/>
       <c r="D147"/>
       <c r="E147"/>
@@ -9925,7 +9925,7 @@
       <c r="U147" s="23"/>
       <c r="V147" s="10"/>
     </row>
-    <row r="148" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C148" s="11"/>
       <c r="D148"/>
       <c r="E148"/>
@@ -9936,7 +9936,7 @@
       <c r="U148" s="23"/>
       <c r="V148" s="10"/>
     </row>
-    <row r="149" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C149" s="11"/>
       <c r="D149"/>
       <c r="E149"/>
@@ -9947,7 +9947,7 @@
       <c r="U149" s="23"/>
       <c r="V149" s="10"/>
     </row>
-    <row r="150" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C150" s="11"/>
       <c r="D150"/>
       <c r="E150"/>
@@ -9958,7 +9958,7 @@
       <c r="U150" s="23"/>
       <c r="V150" s="10"/>
     </row>
-    <row r="151" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C151" s="11"/>
       <c r="D151"/>
       <c r="E151"/>
@@ -9969,7 +9969,7 @@
       <c r="U151" s="23"/>
       <c r="V151" s="10"/>
     </row>
-    <row r="152" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C152" s="11"/>
       <c r="D152"/>
       <c r="E152"/>
@@ -9980,7 +9980,7 @@
       <c r="U152" s="23"/>
       <c r="V152" s="10"/>
     </row>
-    <row r="153" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C153" s="11"/>
       <c r="D153"/>
       <c r="E153"/>
@@ -9991,7 +9991,7 @@
       <c r="U153" s="23"/>
       <c r="V153" s="10"/>
     </row>
-    <row r="154" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C154" s="11"/>
       <c r="D154"/>
       <c r="E154"/>
@@ -10002,7 +10002,7 @@
       <c r="U154" s="23"/>
       <c r="V154" s="10"/>
     </row>
-    <row r="155" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C155" s="11"/>
       <c r="D155"/>
       <c r="E155"/>
@@ -10013,7 +10013,7 @@
       <c r="U155" s="23"/>
       <c r="V155" s="10"/>
     </row>
-    <row r="156" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C156" s="11"/>
       <c r="D156"/>
       <c r="E156"/>
@@ -10024,7 +10024,7 @@
       <c r="U156" s="23"/>
       <c r="V156" s="10"/>
     </row>
-    <row r="157" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C157" s="11"/>
       <c r="D157"/>
       <c r="E157"/>
@@ -10035,7 +10035,7 @@
       <c r="U157" s="23"/>
       <c r="V157" s="10"/>
     </row>
-    <row r="158" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C158" s="11"/>
       <c r="D158"/>
       <c r="E158"/>
@@ -10046,7 +10046,7 @@
       <c r="U158" s="23"/>
       <c r="V158" s="10"/>
     </row>
-    <row r="159" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C159" s="11"/>
       <c r="D159"/>
       <c r="E159"/>
@@ -10057,7 +10057,7 @@
       <c r="U159" s="23"/>
       <c r="V159" s="10"/>
     </row>
-    <row r="160" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C160" s="11"/>
       <c r="D160"/>
       <c r="E160"/>
@@ -10068,7 +10068,7 @@
       <c r="U160" s="23"/>
       <c r="V160" s="10"/>
     </row>
-    <row r="161" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C161" s="11"/>
       <c r="D161"/>
       <c r="E161"/>
@@ -10079,7 +10079,7 @@
       <c r="U161" s="23"/>
       <c r="V161" s="10"/>
     </row>
-    <row r="162" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C162" s="11"/>
       <c r="D162"/>
       <c r="E162"/>
@@ -10090,7 +10090,7 @@
       <c r="U162" s="23"/>
       <c r="V162" s="10"/>
     </row>
-    <row r="163" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C163" s="11"/>
       <c r="D163"/>
       <c r="E163"/>
@@ -10101,7 +10101,7 @@
       <c r="U163" s="23"/>
       <c r="V163" s="10"/>
     </row>
-    <row r="164" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C164" s="11"/>
       <c r="D164"/>
       <c r="E164"/>
@@ -10112,7 +10112,7 @@
       <c r="U164" s="23"/>
       <c r="V164" s="10"/>
     </row>
-    <row r="165" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C165" s="11"/>
       <c r="D165"/>
       <c r="E165"/>
@@ -10123,7 +10123,7 @@
       <c r="U165" s="23"/>
       <c r="V165" s="10"/>
     </row>
-    <row r="166" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C166" s="11"/>
       <c r="D166"/>
       <c r="E166"/>
@@ -10134,7 +10134,7 @@
       <c r="U166" s="23"/>
       <c r="V166" s="10"/>
     </row>
-    <row r="167" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C167" s="11"/>
       <c r="D167"/>
       <c r="E167"/>
@@ -10145,7 +10145,7 @@
       <c r="U167" s="23"/>
       <c r="V167" s="10"/>
     </row>
-    <row r="168" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C168" s="11"/>
       <c r="D168"/>
       <c r="E168"/>
@@ -10156,7 +10156,7 @@
       <c r="U168" s="23"/>
       <c r="V168" s="10"/>
     </row>
-    <row r="169" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C169" s="11"/>
       <c r="D169"/>
       <c r="E169"/>
@@ -10167,7 +10167,7 @@
       <c r="U169" s="23"/>
       <c r="V169" s="10"/>
     </row>
-    <row r="170" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C170" s="11"/>
       <c r="D170"/>
       <c r="E170"/>
@@ -10178,7 +10178,7 @@
       <c r="U170" s="23"/>
       <c r="V170" s="10"/>
     </row>
-    <row r="171" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C171" s="11"/>
       <c r="D171"/>
       <c r="E171"/>
@@ -10189,7 +10189,7 @@
       <c r="U171" s="23"/>
       <c r="V171" s="10"/>
     </row>
-    <row r="172" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C172" s="11"/>
       <c r="D172"/>
       <c r="E172"/>
@@ -10200,7 +10200,7 @@
       <c r="U172" s="23"/>
       <c r="V172" s="10"/>
     </row>
-    <row r="173" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C173" s="11"/>
       <c r="D173"/>
       <c r="E173"/>
@@ -10211,7 +10211,7 @@
       <c r="U173" s="23"/>
       <c r="V173" s="10"/>
     </row>
-    <row r="174" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C174" s="11"/>
       <c r="D174"/>
       <c r="E174"/>
@@ -10222,7 +10222,7 @@
       <c r="U174" s="23"/>
       <c r="V174" s="10"/>
     </row>
-    <row r="175" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C175" s="11"/>
       <c r="D175"/>
       <c r="E175"/>
@@ -10233,7 +10233,7 @@
       <c r="U175" s="23"/>
       <c r="V175" s="10"/>
     </row>
-    <row r="176" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C176" s="11"/>
       <c r="D176"/>
       <c r="E176"/>
@@ -10244,7 +10244,7 @@
       <c r="U176" s="23"/>
       <c r="V176" s="10"/>
     </row>
-    <row r="177" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C177" s="11"/>
       <c r="D177"/>
       <c r="E177"/>
@@ -10255,7 +10255,7 @@
       <c r="U177" s="23"/>
       <c r="V177" s="10"/>
     </row>
-    <row r="178" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C178" s="11"/>
       <c r="D178"/>
       <c r="E178"/>
@@ -10266,7 +10266,7 @@
       <c r="U178" s="23"/>
       <c r="V178" s="10"/>
     </row>
-    <row r="179" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C179" s="11"/>
       <c r="D179"/>
       <c r="E179"/>
@@ -10277,7 +10277,7 @@
       <c r="U179" s="23"/>
       <c r="V179" s="10"/>
     </row>
-    <row r="180" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C180" s="11"/>
       <c r="D180"/>
       <c r="E180"/>
@@ -10288,7 +10288,7 @@
       <c r="U180" s="23"/>
       <c r="V180" s="10"/>
     </row>
-    <row r="181" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C181" s="11"/>
       <c r="D181"/>
       <c r="E181"/>
@@ -10299,7 +10299,7 @@
       <c r="U181" s="23"/>
       <c r="V181" s="10"/>
     </row>
-    <row r="182" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C182" s="11"/>
       <c r="D182"/>
       <c r="E182"/>
@@ -10310,7 +10310,7 @@
       <c r="U182" s="23"/>
       <c r="V182" s="10"/>
     </row>
-    <row r="183" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C183" s="11"/>
       <c r="D183"/>
       <c r="E183"/>
@@ -10321,7 +10321,7 @@
       <c r="U183" s="23"/>
       <c r="V183" s="10"/>
     </row>
-    <row r="184" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C184" s="11"/>
       <c r="D184"/>
       <c r="E184"/>
@@ -10332,7 +10332,7 @@
       <c r="U184" s="23"/>
       <c r="V184" s="10"/>
     </row>
-    <row r="185" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C185" s="11"/>
       <c r="D185"/>
       <c r="E185"/>
@@ -10343,7 +10343,7 @@
       <c r="U185" s="23"/>
       <c r="V185" s="10"/>
     </row>
-    <row r="186" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C186" s="11"/>
       <c r="D186"/>
       <c r="E186"/>
@@ -10354,7 +10354,7 @@
       <c r="U186" s="23"/>
       <c r="V186" s="10"/>
     </row>
-    <row r="187" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C187" s="11"/>
       <c r="D187"/>
       <c r="E187"/>
@@ -10365,7 +10365,7 @@
       <c r="U187" s="23"/>
       <c r="V187" s="10"/>
     </row>
-    <row r="188" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C188" s="11"/>
       <c r="D188"/>
       <c r="E188"/>
@@ -10376,7 +10376,7 @@
       <c r="U188" s="23"/>
       <c r="V188" s="10"/>
     </row>
-    <row r="189" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C189" s="11"/>
       <c r="D189"/>
       <c r="E189"/>
@@ -10387,7 +10387,7 @@
       <c r="U189" s="23"/>
       <c r="V189" s="10"/>
     </row>
-    <row r="190" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C190" s="11"/>
       <c r="D190"/>
       <c r="E190"/>
@@ -10398,7 +10398,7 @@
       <c r="U190" s="23"/>
       <c r="V190" s="10"/>
     </row>
-    <row r="191" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C191" s="11"/>
       <c r="D191"/>
       <c r="E191"/>
@@ -10409,7 +10409,7 @@
       <c r="U191" s="23"/>
       <c r="V191" s="10"/>
     </row>
-    <row r="192" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C192" s="11"/>
       <c r="D192"/>
       <c r="E192"/>
@@ -10420,7 +10420,7 @@
       <c r="U192" s="23"/>
       <c r="V192" s="10"/>
     </row>
-    <row r="193" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C193" s="11"/>
       <c r="D193"/>
       <c r="E193"/>
@@ -10431,7 +10431,7 @@
       <c r="U193" s="23"/>
       <c r="V193" s="10"/>
     </row>
-    <row r="194" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C194" s="11"/>
       <c r="D194"/>
       <c r="E194"/>
@@ -10442,7 +10442,7 @@
       <c r="U194" s="23"/>
       <c r="V194" s="10"/>
     </row>
-    <row r="195" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C195" s="11"/>
       <c r="D195"/>
       <c r="E195"/>
@@ -10453,7 +10453,7 @@
       <c r="U195" s="23"/>
       <c r="V195" s="10"/>
     </row>
-    <row r="196" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C196" s="11"/>
       <c r="D196"/>
       <c r="E196"/>
@@ -10464,7 +10464,7 @@
       <c r="U196" s="23"/>
       <c r="V196" s="10"/>
     </row>
-    <row r="197" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C197" s="11"/>
       <c r="D197"/>
       <c r="E197"/>
@@ -10475,7 +10475,7 @@
       <c r="U197" s="23"/>
       <c r="V197" s="10"/>
     </row>
-    <row r="198" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C198" s="11"/>
       <c r="D198"/>
       <c r="E198"/>
@@ -10486,7 +10486,7 @@
       <c r="U198" s="23"/>
       <c r="V198" s="10"/>
     </row>
-    <row r="199" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C199" s="11"/>
       <c r="D199"/>
       <c r="E199"/>
@@ -10497,7 +10497,7 @@
       <c r="U199" s="23"/>
       <c r="V199" s="10"/>
     </row>
-    <row r="200" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C200" s="11"/>
       <c r="D200"/>
       <c r="E200"/>
@@ -10508,7 +10508,7 @@
       <c r="U200" s="23"/>
       <c r="V200" s="10"/>
     </row>
-    <row r="201" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C201" s="11"/>
       <c r="D201"/>
       <c r="E201"/>
@@ -10519,7 +10519,7 @@
       <c r="U201" s="23"/>
       <c r="V201" s="10"/>
     </row>
-    <row r="202" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C202" s="11"/>
       <c r="D202"/>
       <c r="E202"/>
@@ -10530,7 +10530,7 @@
       <c r="U202" s="23"/>
       <c r="V202" s="10"/>
     </row>
-    <row r="203" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C203" s="11"/>
       <c r="D203"/>
       <c r="E203"/>
@@ -10541,7 +10541,7 @@
       <c r="U203" s="23"/>
       <c r="V203" s="10"/>
     </row>
-    <row r="204" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C204" s="11"/>
       <c r="D204"/>
       <c r="E204"/>
@@ -10552,7 +10552,7 @@
       <c r="U204" s="23"/>
       <c r="V204" s="10"/>
     </row>
-    <row r="205" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C205" s="11"/>
       <c r="D205"/>
       <c r="E205"/>
@@ -10563,7 +10563,7 @@
       <c r="U205" s="23"/>
       <c r="V205" s="10"/>
     </row>
-    <row r="206" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C206" s="11"/>
       <c r="D206"/>
       <c r="E206"/>
@@ -10574,7 +10574,7 @@
       <c r="U206" s="23"/>
       <c r="V206" s="10"/>
     </row>
-    <row r="207" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C207" s="11"/>
       <c r="D207"/>
       <c r="E207"/>
@@ -10585,7 +10585,7 @@
       <c r="U207" s="23"/>
       <c r="V207" s="10"/>
     </row>
-    <row r="208" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C208" s="11"/>
       <c r="D208"/>
       <c r="E208"/>
@@ -10596,7 +10596,7 @@
       <c r="U208" s="23"/>
       <c r="V208" s="10"/>
     </row>
-    <row r="209" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C209" s="11"/>
       <c r="D209"/>
       <c r="E209"/>
@@ -10607,7 +10607,7 @@
       <c r="U209" s="23"/>
       <c r="V209" s="10"/>
     </row>
-    <row r="210" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C210" s="11"/>
       <c r="D210"/>
       <c r="E210"/>
@@ -10618,7 +10618,7 @@
       <c r="U210" s="23"/>
       <c r="V210" s="10"/>
     </row>
-    <row r="211" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C211" s="11"/>
       <c r="D211"/>
       <c r="E211"/>
@@ -10629,7 +10629,7 @@
       <c r="U211" s="23"/>
       <c r="V211" s="10"/>
     </row>
-    <row r="212" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C212" s="11"/>
       <c r="D212"/>
       <c r="E212"/>
@@ -10640,7 +10640,7 @@
       <c r="U212" s="23"/>
       <c r="V212" s="10"/>
     </row>
-    <row r="213" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C213" s="11"/>
       <c r="D213"/>
       <c r="E213"/>
@@ -10651,7 +10651,7 @@
       <c r="U213" s="23"/>
       <c r="V213" s="10"/>
     </row>
-    <row r="214" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C214" s="11"/>
       <c r="D214"/>
       <c r="E214"/>
@@ -10662,7 +10662,7 @@
       <c r="U214" s="23"/>
       <c r="V214" s="10"/>
     </row>
-    <row r="215" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C215" s="11"/>
       <c r="D215"/>
       <c r="E215"/>
@@ -10673,7 +10673,7 @@
       <c r="U215" s="23"/>
       <c r="V215" s="10"/>
     </row>
-    <row r="216" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C216" s="11"/>
       <c r="D216"/>
       <c r="E216"/>
@@ -10684,7 +10684,7 @@
       <c r="U216" s="23"/>
       <c r="V216" s="10"/>
     </row>
-    <row r="217" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C217" s="11"/>
       <c r="D217"/>
       <c r="E217"/>
@@ -10695,7 +10695,7 @@
       <c r="U217" s="23"/>
       <c r="V217" s="10"/>
     </row>
-    <row r="218" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C218" s="11"/>
       <c r="D218"/>
       <c r="E218"/>
@@ -10706,7 +10706,7 @@
       <c r="U218" s="23"/>
       <c r="V218" s="10"/>
     </row>
-    <row r="219" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C219" s="11"/>
       <c r="D219"/>
       <c r="E219"/>
@@ -10717,7 +10717,7 @@
       <c r="U219" s="23"/>
       <c r="V219" s="10"/>
     </row>
-    <row r="220" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C220" s="11"/>
       <c r="D220"/>
       <c r="E220"/>
@@ -10728,7 +10728,7 @@
       <c r="U220" s="23"/>
       <c r="V220" s="10"/>
     </row>
-    <row r="221" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C221" s="11"/>
       <c r="D221"/>
       <c r="E221"/>
@@ -10739,7 +10739,7 @@
       <c r="U221" s="23"/>
       <c r="V221" s="10"/>
     </row>
-    <row r="222" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C222" s="11"/>
       <c r="D222"/>
       <c r="E222"/>
@@ -10750,7 +10750,7 @@
       <c r="U222" s="23"/>
       <c r="V222" s="10"/>
     </row>
-    <row r="223" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C223" s="11"/>
       <c r="D223"/>
       <c r="E223"/>
@@ -10761,7 +10761,7 @@
       <c r="U223" s="23"/>
       <c r="V223" s="10"/>
     </row>
-    <row r="224" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C224" s="11"/>
       <c r="D224"/>
       <c r="E224"/>
@@ -10772,7 +10772,7 @@
       <c r="U224" s="23"/>
       <c r="V224" s="10"/>
     </row>
-    <row r="225" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C225" s="11"/>
       <c r="D225"/>
       <c r="E225"/>
@@ -10783,7 +10783,7 @@
       <c r="U225" s="23"/>
       <c r="V225" s="10"/>
     </row>
-    <row r="226" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C226" s="11"/>
       <c r="D226"/>
       <c r="E226"/>
@@ -10794,7 +10794,7 @@
       <c r="U226" s="23"/>
       <c r="V226" s="10"/>
     </row>
-    <row r="227" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C227" s="11"/>
       <c r="D227"/>
       <c r="E227"/>
@@ -10805,7 +10805,7 @@
       <c r="U227" s="23"/>
       <c r="V227" s="10"/>
     </row>
-    <row r="228" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C228" s="11"/>
       <c r="D228"/>
       <c r="E228"/>
@@ -10816,7 +10816,7 @@
       <c r="U228" s="23"/>
       <c r="V228" s="10"/>
     </row>
-    <row r="229" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C229" s="11"/>
       <c r="D229"/>
       <c r="E229"/>
@@ -10827,7 +10827,7 @@
       <c r="U229" s="23"/>
       <c r="V229" s="10"/>
     </row>
-    <row r="230" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C230" s="11"/>
       <c r="D230"/>
       <c r="E230"/>
@@ -10838,7 +10838,7 @@
       <c r="U230" s="23"/>
       <c r="V230" s="10"/>
     </row>
-    <row r="231" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C231" s="11"/>
       <c r="D231"/>
       <c r="E231"/>
@@ -10849,7 +10849,7 @@
       <c r="U231" s="23"/>
       <c r="V231" s="10"/>
     </row>
-    <row r="232" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C232" s="11"/>
       <c r="D232"/>
       <c r="E232"/>
@@ -10860,7 +10860,7 @@
       <c r="U232" s="23"/>
       <c r="V232" s="10"/>
     </row>
-    <row r="233" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C233" s="11"/>
       <c r="D233"/>
       <c r="E233"/>
@@ -10871,7 +10871,7 @@
       <c r="U233" s="23"/>
       <c r="V233" s="10"/>
     </row>
-    <row r="234" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C234" s="11"/>
       <c r="D234"/>
       <c r="E234"/>
@@ -10882,7 +10882,7 @@
       <c r="U234" s="23"/>
       <c r="V234" s="10"/>
     </row>
-    <row r="235" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C235" s="11"/>
       <c r="D235"/>
       <c r="E235"/>
@@ -10893,7 +10893,7 @@
       <c r="U235" s="23"/>
       <c r="V235" s="10"/>
     </row>
-    <row r="236" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C236" s="11"/>
       <c r="D236"/>
       <c r="E236"/>
@@ -10904,7 +10904,7 @@
       <c r="U236" s="23"/>
       <c r="V236" s="10"/>
     </row>
-    <row r="237" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C237" s="11"/>
       <c r="D237"/>
       <c r="E237"/>
@@ -10915,7 +10915,7 @@
       <c r="U237" s="23"/>
       <c r="V237" s="10"/>
     </row>
-    <row r="238" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C238" s="11"/>
       <c r="D238"/>
       <c r="E238"/>
@@ -10926,7 +10926,7 @@
       <c r="U238" s="23"/>
       <c r="V238" s="10"/>
     </row>
-    <row r="239" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C239" s="11"/>
       <c r="D239"/>
       <c r="E239"/>
@@ -10937,7 +10937,7 @@
       <c r="U239" s="23"/>
       <c r="V239" s="10"/>
     </row>
-    <row r="240" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C240" s="11"/>
       <c r="D240"/>
       <c r="E240"/>
@@ -10948,7 +10948,7 @@
       <c r="U240" s="23"/>
       <c r="V240" s="10"/>
     </row>
-    <row r="241" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C241" s="11"/>
       <c r="D241"/>
       <c r="E241"/>
@@ -10959,7 +10959,7 @@
       <c r="U241" s="23"/>
       <c r="V241" s="10"/>
     </row>
-    <row r="242" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C242" s="11"/>
       <c r="D242"/>
       <c r="E242"/>
@@ -10970,7 +10970,7 @@
       <c r="U242" s="23"/>
       <c r="V242" s="10"/>
     </row>
-    <row r="243" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C243" s="11"/>
       <c r="D243"/>
       <c r="E243"/>
@@ -10981,7 +10981,7 @@
       <c r="U243" s="23"/>
       <c r="V243" s="10"/>
     </row>
-    <row r="244" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C244" s="11"/>
       <c r="D244"/>
       <c r="E244"/>
@@ -10992,7 +10992,7 @@
       <c r="U244" s="23"/>
       <c r="V244" s="10"/>
     </row>
-    <row r="245" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C245" s="11"/>
       <c r="D245"/>
       <c r="E245"/>
@@ -11003,7 +11003,7 @@
       <c r="U245" s="23"/>
       <c r="V245" s="10"/>
     </row>
-    <row r="246" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C246" s="11"/>
       <c r="D246"/>
       <c r="E246"/>
@@ -11014,7 +11014,7 @@
       <c r="U246" s="23"/>
       <c r="V246" s="10"/>
     </row>
-    <row r="247" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C247" s="11"/>
       <c r="D247"/>
       <c r="E247"/>
@@ -11025,7 +11025,7 @@
       <c r="U247" s="23"/>
       <c r="V247" s="10"/>
     </row>
-    <row r="248" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C248" s="11"/>
       <c r="D248"/>
       <c r="E248"/>
@@ -11036,7 +11036,7 @@
       <c r="U248" s="23"/>
       <c r="V248" s="10"/>
     </row>
-    <row r="249" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C249" s="11"/>
       <c r="D249"/>
       <c r="E249"/>
@@ -11047,7 +11047,7 @@
       <c r="U249" s="23"/>
       <c r="V249" s="10"/>
     </row>
-    <row r="250" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C250" s="11"/>
       <c r="D250"/>
       <c r="E250"/>
@@ -11058,7 +11058,7 @@
       <c r="U250" s="23"/>
       <c r="V250" s="10"/>
     </row>
-    <row r="251" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C251" s="11"/>
       <c r="D251"/>
       <c r="E251"/>
@@ -11069,7 +11069,7 @@
       <c r="U251" s="23"/>
       <c r="V251" s="10"/>
     </row>
-    <row r="252" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C252" s="11"/>
       <c r="D252"/>
       <c r="E252"/>
@@ -11080,7 +11080,7 @@
       <c r="U252" s="23"/>
       <c r="V252" s="10"/>
     </row>
-    <row r="253" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C253" s="11"/>
       <c r="D253"/>
       <c r="E253"/>
@@ -11091,7 +11091,7 @@
       <c r="U253" s="23"/>
       <c r="V253" s="10"/>
     </row>
-    <row r="254" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C254" s="11"/>
       <c r="D254"/>
       <c r="E254"/>
@@ -11102,7 +11102,7 @@
       <c r="U254" s="23"/>
       <c r="V254" s="10"/>
     </row>
-    <row r="255" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C255" s="11"/>
       <c r="D255"/>
       <c r="E255"/>
@@ -11113,7 +11113,7 @@
       <c r="U255" s="23"/>
       <c r="V255" s="10"/>
     </row>
-    <row r="256" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C256" s="11"/>
       <c r="D256"/>
       <c r="E256"/>
@@ -11124,7 +11124,7 @@
       <c r="U256" s="23"/>
       <c r="V256" s="10"/>
     </row>
-    <row r="257" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C257" s="11"/>
       <c r="D257"/>
       <c r="E257"/>
@@ -11135,7 +11135,7 @@
       <c r="U257" s="23"/>
       <c r="V257" s="10"/>
     </row>
-    <row r="258" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C258" s="11"/>
       <c r="D258"/>
       <c r="E258"/>
@@ -11146,7 +11146,7 @@
       <c r="U258" s="23"/>
       <c r="V258" s="10"/>
     </row>
-    <row r="259" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C259" s="11"/>
       <c r="D259"/>
       <c r="E259"/>
@@ -11157,7 +11157,7 @@
       <c r="U259" s="23"/>
       <c r="V259" s="10"/>
     </row>
-    <row r="260" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C260" s="11"/>
       <c r="D260"/>
       <c r="E260"/>
@@ -11168,7 +11168,7 @@
       <c r="U260" s="23"/>
       <c r="V260" s="10"/>
     </row>
-    <row r="261" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C261" s="11"/>
       <c r="D261"/>
       <c r="E261"/>
@@ -11179,7 +11179,7 @@
       <c r="U261" s="23"/>
       <c r="V261" s="10"/>
     </row>
-    <row r="262" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C262" s="11"/>
       <c r="D262"/>
       <c r="E262"/>
@@ -11190,7 +11190,7 @@
       <c r="U262" s="23"/>
       <c r="V262" s="10"/>
     </row>
-    <row r="263" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C263" s="11"/>
       <c r="D263"/>
       <c r="E263"/>
@@ -11201,7 +11201,7 @@
       <c r="U263" s="23"/>
       <c r="V263" s="10"/>
     </row>
-    <row r="264" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C264" s="11"/>
       <c r="D264"/>
       <c r="E264"/>
@@ -11212,7 +11212,7 @@
       <c r="U264" s="23"/>
       <c r="V264" s="10"/>
     </row>
-    <row r="265" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C265" s="11"/>
       <c r="D265"/>
       <c r="E265"/>
@@ -11223,7 +11223,7 @@
       <c r="U265" s="23"/>
       <c r="V265" s="10"/>
     </row>
-    <row r="266" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C266" s="11"/>
       <c r="D266"/>
       <c r="E266"/>
@@ -11234,7 +11234,7 @@
       <c r="U266" s="23"/>
       <c r="V266" s="10"/>
     </row>
-    <row r="267" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C267" s="11"/>
       <c r="D267"/>
       <c r="E267"/>
@@ -11245,7 +11245,7 @@
       <c r="U267" s="23"/>
       <c r="V267" s="10"/>
     </row>
-    <row r="268" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C268" s="11"/>
       <c r="D268"/>
       <c r="E268"/>
@@ -11256,7 +11256,7 @@
       <c r="U268" s="23"/>
       <c r="V268" s="10"/>
     </row>
-    <row r="269" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C269" s="11"/>
       <c r="D269"/>
       <c r="E269"/>
@@ -11267,7 +11267,7 @@
       <c r="U269" s="23"/>
       <c r="V269" s="10"/>
     </row>
-    <row r="270" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C270" s="11"/>
       <c r="D270"/>
       <c r="E270"/>
@@ -11278,7 +11278,7 @@
       <c r="U270" s="23"/>
       <c r="V270" s="10"/>
     </row>
-    <row r="271" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C271" s="11"/>
       <c r="D271"/>
       <c r="E271"/>
@@ -11289,7 +11289,7 @@
       <c r="U271" s="23"/>
       <c r="V271" s="10"/>
     </row>
-    <row r="272" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C272" s="11"/>
       <c r="D272"/>
       <c r="E272"/>
@@ -11300,7 +11300,7 @@
       <c r="U272" s="23"/>
       <c r="V272" s="10"/>
     </row>
-    <row r="273" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C273" s="11"/>
       <c r="D273"/>
       <c r="E273"/>
@@ -11311,7 +11311,7 @@
       <c r="U273" s="23"/>
       <c r="V273" s="10"/>
     </row>
-    <row r="274" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C274" s="11"/>
       <c r="D274"/>
       <c r="E274"/>
@@ -11322,7 +11322,7 @@
       <c r="U274" s="23"/>
       <c r="V274" s="10"/>
     </row>
-    <row r="275" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C275" s="11"/>
       <c r="D275"/>
       <c r="E275"/>
@@ -11333,7 +11333,7 @@
       <c r="U275" s="23"/>
       <c r="V275" s="10"/>
     </row>
-    <row r="276" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C276" s="11"/>
       <c r="D276"/>
       <c r="E276"/>
@@ -11344,7 +11344,7 @@
       <c r="U276" s="23"/>
       <c r="V276" s="10"/>
     </row>
-    <row r="277" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C277" s="11"/>
       <c r="D277"/>
       <c r="E277"/>
@@ -11355,7 +11355,7 @@
       <c r="U277" s="23"/>
       <c r="V277" s="10"/>
     </row>
-    <row r="278" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C278" s="11"/>
       <c r="D278"/>
       <c r="E278"/>
@@ -11366,7 +11366,7 @@
       <c r="U278" s="23"/>
       <c r="V278" s="10"/>
     </row>
-    <row r="279" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C279" s="11"/>
       <c r="D279"/>
       <c r="E279"/>
@@ -11377,7 +11377,7 @@
       <c r="U279" s="23"/>
       <c r="V279" s="10"/>
     </row>
-    <row r="280" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C280" s="11"/>
       <c r="D280"/>
       <c r="E280"/>
@@ -11388,7 +11388,7 @@
       <c r="U280" s="23"/>
       <c r="V280" s="10"/>
     </row>
-    <row r="281" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C281" s="11"/>
       <c r="D281"/>
       <c r="E281"/>
@@ -11399,7 +11399,7 @@
       <c r="U281" s="23"/>
       <c r="V281" s="10"/>
     </row>
-    <row r="282" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C282" s="11"/>
       <c r="D282"/>
       <c r="E282"/>
@@ -11410,7 +11410,7 @@
       <c r="U282" s="23"/>
       <c r="V282" s="10"/>
     </row>
-    <row r="283" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C283" s="11"/>
       <c r="D283"/>
       <c r="E283"/>
@@ -11421,7 +11421,7 @@
       <c r="U283" s="23"/>
       <c r="V283" s="10"/>
     </row>
-    <row r="284" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C284" s="11"/>
       <c r="D284"/>
       <c r="E284"/>
@@ -11432,7 +11432,7 @@
       <c r="U284" s="23"/>
       <c r="V284" s="10"/>
     </row>
-    <row r="285" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C285" s="11"/>
       <c r="D285"/>
       <c r="E285"/>
@@ -11443,7 +11443,7 @@
       <c r="U285" s="23"/>
       <c r="V285" s="10"/>
     </row>
-    <row r="286" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C286" s="11"/>
       <c r="D286"/>
       <c r="E286"/>
@@ -11454,7 +11454,7 @@
       <c r="U286" s="23"/>
       <c r="V286" s="10"/>
     </row>
-    <row r="287" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C287" s="11"/>
       <c r="D287"/>
       <c r="E287"/>
@@ -11465,7 +11465,7 @@
       <c r="U287" s="23"/>
       <c r="V287" s="10"/>
     </row>
-    <row r="288" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C288" s="11"/>
       <c r="D288"/>
       <c r="E288"/>
@@ -11476,7 +11476,7 @@
       <c r="U288" s="23"/>
       <c r="V288" s="10"/>
     </row>
-    <row r="289" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C289" s="11"/>
       <c r="D289"/>
       <c r="E289"/>
@@ -11487,7 +11487,7 @@
       <c r="U289" s="23"/>
       <c r="V289" s="10"/>
     </row>
-    <row r="290" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C290" s="11"/>
       <c r="D290"/>
       <c r="E290"/>
@@ -11498,7 +11498,7 @@
       <c r="U290" s="23"/>
       <c r="V290" s="10"/>
     </row>
-    <row r="291" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C291" s="11"/>
       <c r="D291"/>
       <c r="E291"/>
@@ -11509,7 +11509,7 @@
       <c r="U291" s="23"/>
       <c r="V291" s="10"/>
     </row>
-    <row r="292" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C292" s="11"/>
       <c r="D292"/>
       <c r="E292"/>
@@ -11520,7 +11520,7 @@
       <c r="U292" s="23"/>
       <c r="V292" s="10"/>
     </row>
-    <row r="293" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C293" s="11"/>
       <c r="D293"/>
       <c r="E293"/>
@@ -11531,7 +11531,7 @@
       <c r="U293" s="23"/>
       <c r="V293" s="10"/>
     </row>
-    <row r="294" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C294" s="11"/>
       <c r="D294"/>
       <c r="E294"/>
@@ -11542,7 +11542,7 @@
       <c r="U294" s="23"/>
       <c r="V294" s="10"/>
     </row>
-    <row r="295" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C295" s="11"/>
       <c r="D295"/>
       <c r="E295"/>
@@ -11553,7 +11553,7 @@
       <c r="U295" s="23"/>
       <c r="V295" s="10"/>
     </row>
-    <row r="296" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C296" s="11"/>
       <c r="D296"/>
       <c r="E296"/>
@@ -11564,7 +11564,7 @@
       <c r="U296" s="23"/>
       <c r="V296" s="10"/>
     </row>
-    <row r="297" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C297" s="11"/>
       <c r="D297"/>
       <c r="E297"/>
@@ -11575,7 +11575,7 @@
       <c r="U297" s="23"/>
       <c r="V297" s="10"/>
     </row>
-    <row r="298" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C298" s="11"/>
       <c r="D298"/>
       <c r="E298"/>
@@ -11586,7 +11586,7 @@
       <c r="U298" s="23"/>
       <c r="V298" s="10"/>
     </row>
-    <row r="299" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C299" s="11"/>
       <c r="D299"/>
       <c r="E299"/>
@@ -11597,7 +11597,7 @@
       <c r="U299" s="23"/>
       <c r="V299" s="10"/>
     </row>
-    <row r="300" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C300" s="11"/>
       <c r="D300"/>
       <c r="E300"/>
@@ -11608,7 +11608,7 @@
       <c r="U300" s="23"/>
       <c r="V300" s="10"/>
     </row>
-    <row r="301" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C301" s="11"/>
       <c r="D301"/>
       <c r="E301"/>
@@ -11619,7 +11619,7 @@
       <c r="U301" s="23"/>
       <c r="V301" s="10"/>
     </row>
-    <row r="302" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C302" s="11"/>
       <c r="D302"/>
       <c r="E302"/>
@@ -11630,7 +11630,7 @@
       <c r="U302" s="23"/>
       <c r="V302" s="10"/>
     </row>
-    <row r="303" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C303" s="11"/>
       <c r="D303"/>
       <c r="E303"/>
@@ -11641,7 +11641,7 @@
       <c r="U303" s="23"/>
       <c r="V303" s="10"/>
     </row>
-    <row r="304" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C304" s="11"/>
       <c r="D304"/>
       <c r="E304"/>
@@ -11652,7 +11652,7 @@
       <c r="U304" s="23"/>
       <c r="V304" s="10"/>
     </row>
-    <row r="305" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C305" s="11"/>
       <c r="D305"/>
       <c r="E305"/>
@@ -11663,7 +11663,7 @@
       <c r="U305" s="23"/>
       <c r="V305" s="10"/>
     </row>
-    <row r="306" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C306" s="11"/>
       <c r="D306"/>
       <c r="E306"/>
@@ -11674,7 +11674,7 @@
       <c r="U306" s="23"/>
       <c r="V306" s="10"/>
     </row>
-    <row r="307" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C307" s="11"/>
       <c r="D307"/>
       <c r="E307"/>
@@ -11685,7 +11685,7 @@
       <c r="U307" s="23"/>
       <c r="V307" s="10"/>
     </row>
-    <row r="308" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C308" s="11"/>
       <c r="D308"/>
       <c r="E308"/>
@@ -11696,7 +11696,7 @@
       <c r="U308" s="23"/>
       <c r="V308" s="10"/>
     </row>
-    <row r="309" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C309" s="11"/>
       <c r="D309"/>
       <c r="E309"/>
@@ -11707,7 +11707,7 @@
       <c r="U309" s="23"/>
       <c r="V309" s="10"/>
     </row>
-    <row r="310" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C310" s="11"/>
       <c r="D310"/>
       <c r="E310"/>
@@ -11718,7 +11718,7 @@
       <c r="U310" s="23"/>
       <c r="V310" s="10"/>
     </row>
-    <row r="311" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C311" s="11"/>
       <c r="D311"/>
       <c r="E311"/>
@@ -11729,7 +11729,7 @@
       <c r="U311" s="23"/>
       <c r="V311" s="10"/>
     </row>
-    <row r="312" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C312" s="11"/>
       <c r="D312"/>
       <c r="E312"/>
@@ -11740,7 +11740,7 @@
       <c r="U312" s="23"/>
       <c r="V312" s="10"/>
     </row>
-    <row r="313" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C313" s="11"/>
       <c r="D313"/>
       <c r="E313"/>
@@ -11751,7 +11751,7 @@
       <c r="U313" s="23"/>
       <c r="V313" s="10"/>
     </row>
-    <row r="314" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C314" s="11"/>
       <c r="D314"/>
       <c r="E314"/>
@@ -11762,7 +11762,7 @@
       <c r="U314" s="23"/>
       <c r="V314" s="10"/>
     </row>
-    <row r="315" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C315" s="11"/>
       <c r="D315"/>
       <c r="E315"/>
@@ -11773,7 +11773,7 @@
       <c r="U315" s="23"/>
       <c r="V315" s="10"/>
     </row>
-    <row r="316" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C316" s="11"/>
       <c r="D316"/>
       <c r="E316"/>
@@ -11784,7 +11784,7 @@
       <c r="U316" s="23"/>
       <c r="V316" s="10"/>
     </row>
-    <row r="317" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C317" s="11"/>
       <c r="D317"/>
       <c r="E317"/>
@@ -11795,7 +11795,7 @@
       <c r="U317" s="23"/>
       <c r="V317" s="10"/>
     </row>
-    <row r="318" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C318" s="12"/>
       <c r="D318"/>
       <c r="E318"/>
@@ -11806,7 +11806,7 @@
       <c r="U318" s="23"/>
       <c r="V318" s="10"/>
     </row>
-    <row r="319" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C319" s="12"/>
       <c r="D319"/>
       <c r="E319"/>
@@ -11817,7 +11817,7 @@
       <c r="U319" s="23"/>
       <c r="V319" s="10"/>
     </row>
-    <row r="320" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C320" s="12"/>
       <c r="D320"/>
       <c r="E320"/>
@@ -11828,7 +11828,7 @@
       <c r="U320" s="23"/>
       <c r="V320" s="10"/>
     </row>
-    <row r="321" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C321" s="12"/>
       <c r="D321"/>
       <c r="E321"/>
@@ -11839,7 +11839,7 @@
       <c r="U321" s="23"/>
       <c r="V321" s="10"/>
     </row>
-    <row r="322" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C322" s="12"/>
       <c r="D322"/>
       <c r="E322"/>
@@ -11850,7 +11850,7 @@
       <c r="U322" s="23"/>
       <c r="V322" s="10"/>
     </row>
-    <row r="323" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C323" s="12"/>
       <c r="D323"/>
       <c r="E323"/>
@@ -11861,7 +11861,7 @@
       <c r="U323" s="23"/>
       <c r="V323" s="10"/>
     </row>
-    <row r="324" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C324" s="12"/>
       <c r="D324"/>
       <c r="E324"/>
@@ -11872,7 +11872,7 @@
       <c r="U324" s="23"/>
       <c r="V324" s="10"/>
     </row>
-    <row r="325" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C325" s="12"/>
       <c r="D325"/>
       <c r="E325"/>
@@ -11883,7 +11883,7 @@
       <c r="U325" s="23"/>
       <c r="V325" s="10"/>
     </row>
-    <row r="326" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C326" s="12"/>
       <c r="D326"/>
       <c r="E326"/>
@@ -11894,7 +11894,7 @@
       <c r="U326" s="23"/>
       <c r="V326" s="10"/>
     </row>
-    <row r="327" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C327" s="12"/>
       <c r="D327"/>
       <c r="E327"/>
@@ -11905,7 +11905,7 @@
       <c r="U327" s="23"/>
       <c r="V327" s="10"/>
     </row>
-    <row r="328" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C328" s="12"/>
       <c r="D328"/>
       <c r="E328"/>
@@ -11916,7 +11916,7 @@
       <c r="U328" s="23"/>
       <c r="V328" s="10"/>
     </row>
-    <row r="329" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C329" s="12"/>
       <c r="D329"/>
       <c r="E329"/>
@@ -11927,7 +11927,7 @@
       <c r="U329" s="23"/>
       <c r="V329" s="10"/>
     </row>
-    <row r="330" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C330" s="12"/>
       <c r="D330"/>
       <c r="E330"/>
@@ -11938,7 +11938,7 @@
       <c r="U330" s="23"/>
       <c r="V330" s="10"/>
     </row>
-    <row r="331" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C331" s="12"/>
       <c r="D331"/>
       <c r="E331"/>
@@ -11949,7 +11949,7 @@
       <c r="U331" s="23"/>
       <c r="V331" s="10"/>
     </row>
-    <row r="332" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C332" s="12"/>
       <c r="D332"/>
       <c r="E332"/>
@@ -11960,7 +11960,7 @@
       <c r="U332" s="23"/>
       <c r="V332" s="10"/>
     </row>
-    <row r="333" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C333" s="12"/>
       <c r="D333"/>
       <c r="E333"/>
@@ -11971,7 +11971,7 @@
       <c r="U333" s="23"/>
       <c r="V333" s="10"/>
     </row>
-    <row r="334" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C334" s="12"/>
       <c r="D334"/>
       <c r="E334"/>
@@ -11982,7 +11982,7 @@
       <c r="U334" s="23"/>
       <c r="V334" s="10"/>
     </row>
-    <row r="335" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C335" s="12"/>
       <c r="D335"/>
       <c r="E335"/>
@@ -11993,7 +11993,7 @@
       <c r="U335" s="23"/>
       <c r="V335" s="10"/>
     </row>
-    <row r="336" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C336" s="12"/>
       <c r="D336"/>
       <c r="E336"/>
@@ -12004,7 +12004,7 @@
       <c r="U336" s="23"/>
       <c r="V336" s="10"/>
     </row>
-    <row r="337" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C337" s="12"/>
       <c r="D337"/>
       <c r="E337"/>
@@ -12015,7 +12015,7 @@
       <c r="U337" s="23"/>
       <c r="V337" s="10"/>
     </row>
-    <row r="338" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="338" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C338" s="12"/>
       <c r="D338"/>
       <c r="E338"/>
@@ -12026,7 +12026,7 @@
       <c r="U338" s="23"/>
       <c r="V338" s="10"/>
     </row>
-    <row r="339" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="339" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C339" s="12"/>
       <c r="D339"/>
       <c r="E339"/>
@@ -12037,7 +12037,7 @@
       <c r="U339" s="23"/>
       <c r="V339" s="10"/>
     </row>
-    <row r="340" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="340" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C340" s="12"/>
       <c r="D340"/>
       <c r="E340"/>
@@ -12048,7 +12048,7 @@
       <c r="U340" s="23"/>
       <c r="V340" s="10"/>
     </row>
-    <row r="341" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C341" s="12"/>
       <c r="D341"/>
       <c r="E341"/>
@@ -12059,7 +12059,7 @@
       <c r="U341" s="23"/>
       <c r="V341" s="10"/>
     </row>
-    <row r="342" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C342" s="12"/>
       <c r="D342"/>
       <c r="E342"/>
@@ -12070,7 +12070,7 @@
       <c r="U342" s="23"/>
       <c r="V342" s="10"/>
     </row>
-    <row r="343" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C343" s="12"/>
       <c r="D343"/>
       <c r="E343"/>
@@ -12081,7 +12081,7 @@
       <c r="U343" s="23"/>
       <c r="V343" s="10"/>
     </row>
-    <row r="344" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="344" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C344" s="12"/>
       <c r="D344"/>
       <c r="E344"/>
@@ -12092,7 +12092,7 @@
       <c r="U344" s="23"/>
       <c r="V344" s="10"/>
     </row>
-    <row r="345" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C345" s="12"/>
       <c r="D345"/>
       <c r="E345"/>
@@ -12103,7 +12103,7 @@
       <c r="U345" s="23"/>
       <c r="V345" s="10"/>
     </row>
-    <row r="346" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="346" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C346" s="11"/>
       <c r="D346"/>
       <c r="E346"/>
@@ -12114,7 +12114,7 @@
       <c r="U346" s="23"/>
       <c r="V346" s="10"/>
     </row>
-    <row r="347" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="347" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C347" s="11"/>
       <c r="D347"/>
       <c r="E347"/>
@@ -12125,7 +12125,7 @@
       <c r="U347" s="23"/>
       <c r="V347" s="10"/>
     </row>
-    <row r="348" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="348" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C348" s="11"/>
       <c r="D348"/>
       <c r="E348"/>
@@ -12136,7 +12136,7 @@
       <c r="U348" s="23"/>
       <c r="V348" s="10"/>
     </row>
-    <row r="349" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C349" s="11"/>
       <c r="D349"/>
       <c r="E349"/>
@@ -12147,7 +12147,7 @@
       <c r="U349" s="23"/>
       <c r="V349" s="10"/>
     </row>
-    <row r="350" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="350" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C350" s="11"/>
       <c r="D350"/>
       <c r="E350"/>
@@ -12158,7 +12158,7 @@
       <c r="U350" s="23"/>
       <c r="V350" s="10"/>
     </row>
-    <row r="351" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="351" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C351" s="11"/>
       <c r="D351"/>
       <c r="E351"/>
@@ -12169,7 +12169,7 @@
       <c r="U351" s="23"/>
       <c r="V351" s="10"/>
     </row>
-    <row r="352" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="352" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C352" s="11"/>
       <c r="D352"/>
       <c r="E352"/>
@@ -12180,7 +12180,7 @@
       <c r="U352" s="23"/>
       <c r="V352" s="10"/>
     </row>
-    <row r="353" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C353" s="11"/>
       <c r="D353"/>
       <c r="E353"/>
@@ -12191,7 +12191,7 @@
       <c r="U353" s="23"/>
       <c r="V353" s="10"/>
     </row>
-    <row r="354" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C354" s="11"/>
       <c r="D354"/>
       <c r="E354"/>
@@ -12202,7 +12202,7 @@
       <c r="U354" s="23"/>
       <c r="V354" s="10"/>
     </row>
-    <row r="355" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C355" s="11"/>
       <c r="D355"/>
       <c r="E355"/>
@@ -12213,7 +12213,7 @@
       <c r="U355" s="23"/>
       <c r="V355" s="10"/>
     </row>
-    <row r="356" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C356" s="11"/>
       <c r="D356"/>
       <c r="E356"/>
@@ -12224,7 +12224,7 @@
       <c r="U356" s="23"/>
       <c r="V356" s="10"/>
     </row>
-    <row r="357" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C357" s="11"/>
       <c r="D357"/>
       <c r="E357"/>
@@ -12235,7 +12235,7 @@
       <c r="U357" s="23"/>
       <c r="V357" s="10"/>
     </row>
-    <row r="358" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C358" s="11"/>
       <c r="D358"/>
       <c r="E358"/>
@@ -12246,7 +12246,7 @@
       <c r="U358" s="23"/>
       <c r="V358" s="10"/>
     </row>
-    <row r="359" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C359" s="11"/>
       <c r="D359"/>
       <c r="E359"/>
@@ -12257,7 +12257,7 @@
       <c r="U359" s="23"/>
       <c r="V359" s="10"/>
     </row>
-    <row r="360" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C360" s="11"/>
       <c r="D360"/>
       <c r="E360"/>
@@ -12268,7 +12268,7 @@
       <c r="U360" s="23"/>
       <c r="V360" s="10"/>
     </row>
-    <row r="361" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C361" s="11"/>
       <c r="D361"/>
       <c r="E361"/>
@@ -12279,7 +12279,7 @@
       <c r="U361" s="23"/>
       <c r="V361" s="10"/>
     </row>
-    <row r="362" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C362" s="11"/>
       <c r="D362"/>
       <c r="E362"/>
@@ -12290,7 +12290,7 @@
       <c r="U362" s="23"/>
       <c r="V362" s="10"/>
     </row>
-    <row r="363" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C363" s="11"/>
       <c r="D363"/>
       <c r="E363"/>
@@ -12301,7 +12301,7 @@
       <c r="U363" s="23"/>
       <c r="V363" s="10"/>
     </row>
-    <row r="364" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C364" s="13"/>
       <c r="D364"/>
       <c r="E364"/>
@@ -12312,7 +12312,7 @@
       <c r="U364" s="23"/>
       <c r="V364" s="10"/>
     </row>
-    <row r="365" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C365" s="13"/>
       <c r="D365"/>
       <c r="E365"/>
@@ -12323,7 +12323,7 @@
       <c r="U365" s="23"/>
       <c r="V365" s="10"/>
     </row>
-    <row r="366" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C366" s="13"/>
       <c r="D366"/>
       <c r="E366"/>
@@ -12334,7 +12334,7 @@
       <c r="U366" s="23"/>
       <c r="V366" s="10"/>
     </row>
-    <row r="367" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C367" s="13"/>
       <c r="D367"/>
       <c r="E367"/>
@@ -12345,7 +12345,7 @@
       <c r="U367" s="23"/>
       <c r="V367" s="10"/>
     </row>
-    <row r="368" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C368" s="13"/>
       <c r="D368"/>
       <c r="E368"/>
@@ -12356,7 +12356,7 @@
       <c r="U368" s="23"/>
       <c r="V368" s="10"/>
     </row>
-    <row r="369" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C369"/>
       <c r="D369"/>
       <c r="E369"/>
@@ -12367,7 +12367,7 @@
       <c r="U369" s="23"/>
       <c r="V369" s="10"/>
     </row>
-    <row r="370" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C370"/>
       <c r="D370"/>
       <c r="E370"/>
@@ -12378,7 +12378,7 @@
       <c r="U370" s="23"/>
       <c r="V370" s="10"/>
     </row>
-    <row r="371" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C371"/>
       <c r="D371"/>
       <c r="E371"/>
@@ -12389,7 +12389,7 @@
       <c r="U371" s="23"/>
       <c r="V371" s="10"/>
     </row>
-    <row r="372" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C372"/>
       <c r="D372"/>
       <c r="E372"/>
@@ -12400,7 +12400,7 @@
       <c r="U372" s="23"/>
       <c r="V372" s="10"/>
     </row>
-    <row r="373" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C373"/>
       <c r="D373"/>
       <c r="E373"/>
@@ -12411,7 +12411,7 @@
       <c r="U373" s="23"/>
       <c r="V373" s="10"/>
     </row>
-    <row r="374" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C374"/>
       <c r="D374"/>
       <c r="E374"/>
@@ -12422,7 +12422,7 @@
       <c r="U374" s="23"/>
       <c r="V374" s="10"/>
     </row>
-    <row r="375" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="375" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C375"/>
       <c r="D375"/>
       <c r="E375"/>
@@ -12433,7 +12433,7 @@
       <c r="U375" s="23"/>
       <c r="V375" s="10"/>
     </row>
-    <row r="376" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="376" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C376"/>
       <c r="D376"/>
       <c r="E376"/>
@@ -12444,7 +12444,7 @@
       <c r="U376" s="23"/>
       <c r="V376" s="10"/>
     </row>
-    <row r="377" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="377" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C377"/>
       <c r="D377"/>
       <c r="E377"/>
@@ -12455,7 +12455,7 @@
       <c r="U377" s="23"/>
       <c r="V377" s="10"/>
     </row>
-    <row r="378" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C378"/>
       <c r="D378"/>
       <c r="E378"/>
@@ -12466,7 +12466,7 @@
       <c r="U378" s="23"/>
       <c r="V378" s="10"/>
     </row>
-    <row r="379" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C379"/>
       <c r="D379"/>
       <c r="E379"/>
@@ -12477,7 +12477,7 @@
       <c r="U379" s="23"/>
       <c r="V379" s="10"/>
     </row>
-    <row r="380" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C380"/>
       <c r="D380"/>
       <c r="E380"/>
@@ -12488,7 +12488,7 @@
       <c r="U380" s="23"/>
       <c r="V380" s="10"/>
     </row>
-    <row r="381" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C381"/>
       <c r="D381"/>
       <c r="E381"/>
@@ -12499,7 +12499,7 @@
       <c r="U381" s="23"/>
       <c r="V381" s="10"/>
     </row>
-    <row r="382" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C382"/>
       <c r="D382"/>
       <c r="E382"/>
@@ -12510,7 +12510,7 @@
       <c r="U382" s="23"/>
       <c r="V382" s="10"/>
     </row>
-    <row r="383" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C383" s="14"/>
       <c r="D383"/>
       <c r="E383"/>
@@ -12521,7 +12521,7 @@
       <c r="U383" s="23"/>
       <c r="V383" s="10"/>
     </row>
-    <row r="384" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C384"/>
       <c r="D384"/>
       <c r="E384"/>
@@ -12532,7 +12532,7 @@
       <c r="U384" s="23"/>
       <c r="V384" s="10"/>
     </row>
-    <row r="385" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="385" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C385"/>
       <c r="D385" s="11"/>
       <c r="E385"/>
@@ -12543,7 +12543,7 @@
       <c r="U385" s="23"/>
       <c r="V385" s="10"/>
     </row>
-    <row r="386" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="386" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C386"/>
       <c r="D386" s="11"/>
       <c r="E386"/>
@@ -12554,7 +12554,7 @@
       <c r="U386" s="23"/>
       <c r="V386" s="10"/>
     </row>
-    <row r="387" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="387" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C387"/>
       <c r="D387" s="11"/>
       <c r="E387"/>
@@ -12565,7 +12565,7 @@
       <c r="U387" s="23"/>
       <c r="V387" s="10"/>
     </row>
-    <row r="388" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="388" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C388"/>
       <c r="D388" s="11"/>
       <c r="E388"/>
@@ -12576,7 +12576,7 @@
       <c r="U388" s="23"/>
       <c r="V388" s="10"/>
     </row>
-    <row r="389" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="389" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C389"/>
       <c r="D389" s="11"/>
       <c r="E389"/>
@@ -12587,7 +12587,7 @@
       <c r="U389" s="23"/>
       <c r="V389" s="10"/>
     </row>
-    <row r="390" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="390" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C390" s="15"/>
       <c r="D390"/>
       <c r="E390"/>
@@ -12598,7 +12598,7 @@
       <c r="U390" s="23"/>
       <c r="V390" s="10"/>
     </row>
-    <row r="391" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="391" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C391" s="15"/>
       <c r="D391"/>
       <c r="E391"/>
@@ -12609,7 +12609,7 @@
       <c r="U391" s="23"/>
       <c r="V391" s="10"/>
     </row>
-    <row r="392" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="392" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C392" s="15"/>
       <c r="D392"/>
       <c r="E392"/>
@@ -12620,7 +12620,7 @@
       <c r="U392" s="23"/>
       <c r="V392" s="10"/>
     </row>
-    <row r="393" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="393" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C393" s="15"/>
       <c r="D393"/>
       <c r="E393"/>
@@ -12631,7 +12631,7 @@
       <c r="U393" s="23"/>
       <c r="V393" s="10"/>
     </row>
-    <row r="394" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="394" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C394" s="11"/>
       <c r="D394"/>
       <c r="E394"/>
@@ -12642,7 +12642,7 @@
       <c r="U394" s="23"/>
       <c r="V394" s="10"/>
     </row>
-    <row r="395" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="395" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C395" s="11"/>
       <c r="D395"/>
       <c r="E395"/>
@@ -12653,7 +12653,7 @@
       <c r="U395" s="23"/>
       <c r="V395" s="10"/>
     </row>
-    <row r="396" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="396" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C396" s="11"/>
       <c r="D396"/>
       <c r="E396"/>
@@ -12664,7 +12664,7 @@
       <c r="U396" s="23"/>
       <c r="V396" s="10"/>
     </row>
-    <row r="397" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="397" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C397" s="15"/>
       <c r="D397"/>
       <c r="E397"/>
@@ -12675,7 +12675,7 @@
       <c r="U397" s="23"/>
       <c r="V397" s="10"/>
     </row>
-    <row r="398" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="398" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C398" s="15"/>
       <c r="D398"/>
       <c r="E398"/>
@@ -12686,7 +12686,7 @@
       <c r="U398" s="23"/>
       <c r="V398" s="10"/>
     </row>
-    <row r="399" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="399" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C399" s="11"/>
       <c r="D399"/>
       <c r="E399"/>
@@ -12697,7 +12697,7 @@
       <c r="U399" s="23"/>
       <c r="V399" s="10"/>
     </row>
-    <row r="400" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="400" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C400" s="11"/>
       <c r="D400"/>
       <c r="E400"/>
@@ -12708,7 +12708,7 @@
       <c r="U400" s="23"/>
       <c r="V400" s="10"/>
     </row>
-    <row r="401" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="401" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C401" s="11"/>
       <c r="D401"/>
       <c r="E401"/>
@@ -12719,7 +12719,7 @@
       <c r="U401" s="23"/>
       <c r="V401" s="10"/>
     </row>
-    <row r="402" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="402" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C402" s="11"/>
       <c r="D402" s="19"/>
       <c r="E402"/>
@@ -12730,7 +12730,7 @@
       <c r="U402" s="23"/>
       <c r="V402" s="10"/>
     </row>
-    <row r="403" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="403" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C403" s="15"/>
       <c r="D403" s="19"/>
       <c r="E403"/>
@@ -12741,7 +12741,7 @@
       <c r="U403" s="23"/>
       <c r="V403" s="10"/>
     </row>
-    <row r="404" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="404" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C404" s="11"/>
       <c r="D404" s="19"/>
       <c r="E404"/>
@@ -12752,7 +12752,7 @@
       <c r="U404" s="23"/>
       <c r="V404" s="10"/>
     </row>
-    <row r="405" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="405" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C405" s="11"/>
       <c r="D405" s="19"/>
       <c r="E405"/>
@@ -12763,7 +12763,7 @@
       <c r="U405" s="23"/>
       <c r="V405" s="10"/>
     </row>
-    <row r="406" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="406" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C406" s="11"/>
       <c r="D406" s="19"/>
       <c r="E406"/>
@@ -12774,7 +12774,7 @@
       <c r="U406" s="23"/>
       <c r="V406" s="10"/>
     </row>
-    <row r="407" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="407" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C407" s="11"/>
       <c r="D407" s="19"/>
       <c r="E407"/>
@@ -12785,7 +12785,7 @@
       <c r="U407" s="23"/>
       <c r="V407" s="10"/>
     </row>
-    <row r="408" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="408" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C408" s="11"/>
       <c r="D408" s="19"/>
       <c r="E408"/>
@@ -12796,7 +12796,7 @@
       <c r="U408" s="23"/>
       <c r="V408" s="10"/>
     </row>
-    <row r="409" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="409" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C409" s="11"/>
       <c r="D409" s="19"/>
       <c r="E409"/>
@@ -12807,7 +12807,7 @@
       <c r="U409" s="23"/>
       <c r="V409" s="10"/>
     </row>
-    <row r="410" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="410" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C410" s="11"/>
       <c r="D410" s="19"/>
       <c r="E410"/>
@@ -12818,7 +12818,7 @@
       <c r="U410" s="23"/>
       <c r="V410" s="10"/>
     </row>
-    <row r="411" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="411" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C411"/>
       <c r="D411"/>
       <c r="E411"/>
@@ -12829,7 +12829,7 @@
       <c r="U411" s="23"/>
       <c r="V411" s="10"/>
     </row>
-    <row r="412" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="412" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C412"/>
       <c r="D412"/>
       <c r="E412"/>
@@ -12840,7 +12840,7 @@
       <c r="U412" s="23"/>
       <c r="V412" s="10"/>
     </row>
-    <row r="413" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="413" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C413" s="16"/>
       <c r="D413"/>
       <c r="E413"/>
@@ -12851,7 +12851,7 @@
       <c r="U413" s="23"/>
       <c r="V413" s="10"/>
     </row>
-    <row r="414" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="414" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C414" s="16"/>
       <c r="D414"/>
       <c r="E414"/>
@@ -12862,7 +12862,7 @@
       <c r="U414" s="23"/>
       <c r="V414" s="10"/>
     </row>
-    <row r="415" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="415" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C415" s="16"/>
       <c r="D415"/>
       <c r="E415"/>
@@ -12873,7 +12873,7 @@
       <c r="U415" s="23"/>
       <c r="V415" s="10"/>
     </row>
-    <row r="416" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="416" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C416" s="11"/>
       <c r="D416"/>
       <c r="E416"/>
@@ -12884,7 +12884,7 @@
       <c r="U416" s="23"/>
       <c r="V416" s="10"/>
     </row>
-    <row r="417" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="417" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C417" s="15"/>
       <c r="D417"/>
       <c r="E417"/>
@@ -12895,7 +12895,7 @@
       <c r="U417" s="23"/>
       <c r="V417" s="10"/>
     </row>
-    <row r="418" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="418" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C418" s="15"/>
       <c r="D418"/>
       <c r="E418"/>
@@ -12906,7 +12906,7 @@
       <c r="U418" s="23"/>
       <c r="V418" s="10"/>
     </row>
-    <row r="419" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="419" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C419" s="15"/>
       <c r="D419"/>
       <c r="E419"/>
@@ -12917,7 +12917,7 @@
       <c r="U419" s="23"/>
       <c r="V419" s="10"/>
     </row>
-    <row r="420" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="420" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C420" s="15"/>
       <c r="D420"/>
       <c r="E420"/>
@@ -12928,7 +12928,7 @@
       <c r="U420" s="23"/>
       <c r="V420" s="10"/>
     </row>
-    <row r="421" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="421" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C421" s="15"/>
       <c r="D421"/>
       <c r="E421"/>
@@ -12939,7 +12939,7 @@
       <c r="U421" s="23"/>
       <c r="V421" s="10"/>
     </row>
-    <row r="422" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="422" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C422" s="15"/>
       <c r="D422"/>
       <c r="E422"/>
@@ -12950,7 +12950,7 @@
       <c r="U422" s="23"/>
       <c r="V422" s="10"/>
     </row>
-    <row r="423" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="423" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C423" s="15"/>
       <c r="D423"/>
       <c r="E423"/>
@@ -12961,7 +12961,7 @@
       <c r="U423" s="23"/>
       <c r="V423" s="10"/>
     </row>
-    <row r="424" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="424" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C424" s="15"/>
       <c r="D424"/>
       <c r="E424"/>
@@ -12972,7 +12972,7 @@
       <c r="U424" s="23"/>
       <c r="V424" s="10"/>
     </row>
-    <row r="425" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="425" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C425" s="15"/>
       <c r="D425"/>
       <c r="E425"/>
@@ -12983,7 +12983,7 @@
       <c r="U425" s="23"/>
       <c r="V425" s="10"/>
     </row>
-    <row r="426" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="426" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C426" s="15"/>
       <c r="D426"/>
       <c r="E426"/>
@@ -12994,7 +12994,7 @@
       <c r="U426" s="23"/>
       <c r="V426" s="10"/>
     </row>
-    <row r="427" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="427" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C427" s="15"/>
       <c r="D427"/>
       <c r="E427"/>
@@ -13005,7 +13005,7 @@
       <c r="U427" s="23"/>
       <c r="V427" s="10"/>
     </row>
-    <row r="428" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="428" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C428" s="15"/>
       <c r="D428"/>
       <c r="E428"/>
@@ -13016,7 +13016,7 @@
       <c r="U428" s="23"/>
       <c r="V428" s="10"/>
     </row>
-    <row r="429" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="429" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C429" s="15"/>
       <c r="D429"/>
       <c r="E429"/>
@@ -13027,7 +13027,7 @@
       <c r="U429" s="23"/>
       <c r="V429" s="10"/>
     </row>
-    <row r="430" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="430" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C430" s="15"/>
       <c r="D430"/>
       <c r="E430"/>
@@ -13038,7 +13038,7 @@
       <c r="U430" s="23"/>
       <c r="V430" s="10"/>
     </row>
-    <row r="431" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="431" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C431" s="15"/>
       <c r="D431"/>
       <c r="E431"/>
@@ -13049,7 +13049,7 @@
       <c r="U431" s="23"/>
       <c r="V431" s="10"/>
     </row>
-    <row r="432" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="432" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C432" s="15"/>
       <c r="D432"/>
       <c r="E432"/>
@@ -13060,7 +13060,7 @@
       <c r="U432" s="23"/>
       <c r="V432" s="10"/>
     </row>
-    <row r="433" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="433" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C433" s="15"/>
       <c r="D433"/>
       <c r="E433"/>
@@ -13071,7 +13071,7 @@
       <c r="U433" s="23"/>
       <c r="V433" s="10"/>
     </row>
-    <row r="434" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="434" spans="3:22" ht="16" x14ac:dyDescent="0.2">
       <c r="C434" s="17"/>
       <c r="D434" s="20"/>
       <c r="E434"/>
@@ -13082,7 +13082,7 @@
       <c r="U434" s="27"/>
       <c r="V434" s="10"/>
     </row>
-    <row r="435" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="435" spans="3:22" ht="16" x14ac:dyDescent="0.2">
       <c r="C435" s="17"/>
       <c r="D435" s="20"/>
       <c r="E435"/>
@@ -13093,7 +13093,7 @@
       <c r="U435" s="25"/>
       <c r="V435" s="10"/>
     </row>
-    <row r="436" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="436" spans="3:22" ht="16" x14ac:dyDescent="0.2">
       <c r="C436" s="17"/>
       <c r="D436" s="20"/>
       <c r="E436"/>
@@ -13104,7 +13104,7 @@
       <c r="U436" s="25"/>
       <c r="V436" s="10"/>
     </row>
-    <row r="437" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="437" spans="3:22" ht="16" x14ac:dyDescent="0.2">
       <c r="C437" s="17"/>
       <c r="D437" s="20"/>
       <c r="E437"/>
@@ -13115,7 +13115,7 @@
       <c r="U437" s="25"/>
       <c r="V437" s="10"/>
     </row>
-    <row r="438" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="438" spans="3:22" ht="16" x14ac:dyDescent="0.2">
       <c r="C438" s="17"/>
       <c r="D438" s="20"/>
       <c r="E438"/>
@@ -13126,7 +13126,7 @@
       <c r="U438" s="25"/>
       <c r="V438" s="10"/>
     </row>
-    <row r="439" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="439" spans="3:22" ht="16" x14ac:dyDescent="0.2">
       <c r="C439" s="17"/>
       <c r="D439" s="20"/>
       <c r="E439"/>
@@ -13137,7 +13137,7 @@
       <c r="U439" s="26"/>
       <c r="V439" s="10"/>
     </row>
-    <row r="440" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="440" spans="3:22" ht="16" x14ac:dyDescent="0.2">
       <c r="C440" s="18"/>
       <c r="D440" s="20"/>
       <c r="E440"/>

</xml_diff>